<commit_message>
Creande escena y parametros mejorados
</commit_message>
<xml_diff>
--- a/escena.xlsx
+++ b/escena.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmed\Downloads\TemporalUniandes\SextoSemestre\Análisis_Inteligente_De_Señales_Y_Sistemas\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF73D228-9FDE-48F0-8260-06379BF21F83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF18F0D8-FA9E-40ED-BB25-44E55D39096E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{944E0823-291F-4AD7-8EBC-794DB4737F42}"/>
   </bookViews>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15280E6B-541A-49E6-BF39-D1593C33B868}">
-  <dimension ref="B1:F22"/>
+  <dimension ref="B1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C3" s="3">
         <v>-10</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C9" s="4">
         <v>5</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C10" s="4">
         <v>-5</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="C11" s="4">
         <v>5</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="C12" s="4">
         <v>10</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="C13" s="4">
         <v>-5</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="C14" s="4">
         <v>-10</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
-        <v>-5</v>
+        <v>-7.5</v>
       </c>
       <c r="C15" s="4">
         <v>5</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
-        <v>-5</v>
+        <v>-7.5</v>
       </c>
       <c r="C16" s="4">
         <v>10</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <v>-5</v>
+        <v>-7.5</v>
       </c>
       <c r="C17" s="4">
         <v>-5</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
-        <v>-5</v>
+        <v>-7.5</v>
       </c>
       <c r="C18" s="4">
         <v>-10</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
-        <v>-10</v>
+        <v>-12.5</v>
       </c>
       <c r="C19" s="4">
         <v>5</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <v>-10</v>
+        <v>-12.5</v>
       </c>
       <c r="C20" s="4">
         <v>10</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
-        <v>-10</v>
+        <v>-12.5</v>
       </c>
       <c r="C21" s="4">
         <v>-5</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
-        <v>-10</v>
+        <v>-12.5</v>
       </c>
       <c r="C22" s="4">
         <v>-10</v>
@@ -786,6 +786,312 @@
         <v>0.9</v>
       </c>
       <c r="F22" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>-2.5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F23" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F24" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>-7.5</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F25" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>-12.5</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F26" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F27" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>-5</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F28" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F29" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F30" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C31" s="4">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F31" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="C32" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F32" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F33" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F34" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="C35" s="4">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F35" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="C36" s="4">
+        <v>10</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F36" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C37" s="4">
+        <v>-15</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F37" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C38" s="4">
+        <v>-15</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F38" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>-2.5</v>
+      </c>
+      <c r="C39" s="4">
+        <v>-15</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F39" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>-7.5</v>
+      </c>
+      <c r="C40" s="4">
+        <v>-15</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F40" s="2">
         <v>40000</v>
       </c>
     </row>

</xml_diff>